<commit_message>
Updated the option calc and added description
git-tfs-id: [http://szvptemfou01:8080/tfs/DefaultCollection]$/FW SVI FF Releases/Release3/FIRMWARE;C92077
</commit_message>
<xml_diff>
--- a/FIRMWARE/tasks/control/TuneStudyOptions.xlsx
+++ b/FIRMWARE/tasks/control/TuneStudyOptions.xlsx
@@ -1,30 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\204061827\TFS\SVIFF_Releases\Release3\FIRMWARE\tasks\control\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\204061827\TFSSC\Workspaces\FW_SVI_FF_Releases\Release3\FIRMWARE\tasks\control\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A1F4486-E53E-4F43-A631-DACA96B481E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8055"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Legend and use" sheetId="2" r:id="rId1"/>
+    <sheet name="Description and calc" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
   <si>
     <t>Bit Num</t>
   </si>
@@ -98,9 +109,6 @@
     <t>1=start with poscomp=15 (COMP_BASE), 0=with existing poscomp</t>
   </si>
   <si>
-    <t>1 looks pretty bad in my experiments</t>
-  </si>
-  <si>
     <t>1=At end of initial stabilization effort, add wait for stable position and pressure</t>
   </si>
   <si>
@@ -113,9 +121,6 @@
     <t>Doesn't look to make much difference</t>
   </si>
   <si>
-    <t>Surprisingly, 0 gives more consistent poscomp</t>
-  </si>
-  <si>
     <t>Applies only to valves with very small P</t>
   </si>
   <si>
@@ -129,13 +134,67 @@
   </si>
   <si>
     <t>Input to SA 130.15-&gt;</t>
+  </si>
+  <si>
+    <t>1 tends to produce lower P but step test looks similar. Repeatability appears worse</t>
+  </si>
+  <si>
+    <t>1 appears to improve consistency but looked not good in my experiments</t>
+  </si>
+  <si>
+    <t>UseSmoothedPositionForPosComp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1=Use smoothed (1st-order filtered) position, 0=instant. </t>
+  </si>
+  <si>
+    <t>UseSmoothedPositionForStep</t>
+  </si>
+  <si>
+    <t>1 requires UseActualPosDiffForPoscomp=1 to have effect. Affects valve swing</t>
+  </si>
+  <si>
+    <t>UsePrelimPosComp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doesn't appear to improve results </t>
+  </si>
+  <si>
+    <t>Provides a small stabilize effort. Slows the procees down</t>
+  </si>
+  <si>
+    <t>1=Update poscomp along with other parameters</t>
+  </si>
+  <si>
+    <t>Color coding:</t>
+  </si>
+  <si>
+    <t>Want to evaluate</t>
+  </si>
+  <si>
+    <t>Most likely, bad idea</t>
+  </si>
+  <si>
+    <t>Not of high importance</t>
+  </si>
+  <si>
+    <t>How to use:</t>
+  </si>
+  <si>
+    <t>Enter 1 in each option cell in col. D you want to activate</t>
+  </si>
+  <si>
+    <t>Cell E1 has the number to punch in command 130.15 F1.</t>
+  </si>
+  <si>
+    <t>Column D will have 1's for the options in effect</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,8 +227,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -188,6 +253,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -201,7 +284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -209,6 +292,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,11 +575,69 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{379C3635-3FB2-4EC1-BCDD-874929F6FD83}">
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,17 +650,17 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D1" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E1" s="3">
         <f>SUMPRODUCT(C3:C34, E3:E34)</f>
-        <v>452</v>
+        <v>136</v>
       </c>
       <c r="F1" s="4">
-        <v>452</v>
+        <v>1348</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -535,7 +680,7 @@
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>15</v>
@@ -545,7 +690,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B3">
@@ -566,6 +711,9 @@
       <c r="G3" t="s">
         <v>16</v>
       </c>
+      <c r="H3" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -590,11 +738,11 @@
         <v>17</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B5">
@@ -608,9 +756,6 @@
         <f t="shared" si="1"/>
         <v>0004</v>
       </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
       <c r="F5">
         <f>IF(_xlfn.BITAND(F$1,C5)&gt;0,1,"")</f>
         <v>1</v>
@@ -618,9 +763,12 @@
       <c r="G5" t="s">
         <v>18</v>
       </c>
+      <c r="H5" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B6">
@@ -634,6 +782,9 @@
         <f t="shared" si="1"/>
         <v>0008</v>
       </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
       <c r="F6" t="str">
         <f t="shared" ref="F6:F15" si="2">IF(_xlfn.BITAND(F$1,C6)&gt;0,1,"")</f>
         <v/>
@@ -641,9 +792,6 @@
       <c r="G6" t="s">
         <v>19</v>
       </c>
-      <c r="H6" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -668,7 +816,7 @@
         <v>20</v>
       </c>
       <c r="H7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -694,11 +842,11 @@
         <v>21</v>
       </c>
       <c r="H8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B9">
@@ -712,22 +860,19 @@
         <f t="shared" si="1"/>
         <v>0040</v>
       </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
       <c r="F9">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B10">
@@ -744,16 +889,16 @@
       <c r="E10">
         <v>1</v>
       </c>
-      <c r="F10">
+      <c r="F10" t="str">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="G10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B11">
@@ -767,19 +912,16 @@
         <f t="shared" si="1"/>
         <v>0100</v>
       </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
       <c r="F11">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B12">
@@ -801,10 +943,13 @@
         <v>23</v>
       </c>
       <c r="H12" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="B13">
         <v>10</v>
       </c>
@@ -816,12 +961,21 @@
         <f t="shared" si="1"/>
         <v>0400</v>
       </c>
-      <c r="F13" t="str">
+      <c r="F13">
         <f t="shared" si="2"/>
-        <v/>
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="B14">
         <v>11</v>
       </c>
@@ -837,8 +991,17 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
+      <c r="G14" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>39</v>
+      </c>
       <c r="B15">
         <v>12</v>
       </c>
@@ -853,6 +1016,12 @@
       <c r="F15" t="str">
         <f t="shared" si="2"/>
         <v/>
+      </c>
+      <c r="G15" t="s">
+        <v>42</v>
+      </c>
+      <c r="H15" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made all intended deviations in autotune runtime-configurable and disabled by default. Command 129.15 reads, and factory command 130.15 writes any of the parameters. A calculator spreadsheet for bit options is provided/modified accordingly
git-tfs-id: [http://szvptemfou01:8080/tfs/DefaultCollection]$/FW SVI FF Releases/Release3/FIRMWARE;C94698
</commit_message>
<xml_diff>
--- a/FIRMWARE/tasks/control/TuneStudyOptions.xlsx
+++ b/FIRMWARE/tasks/control/TuneStudyOptions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\204061827\TFSSC\Workspaces\FW_SVI_FF_Releases\Release3\FIRMWARE\tasks\control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A1F4486-E53E-4F43-A631-DACA96B481E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9854255-B3C5-415E-90DF-0E2C71715606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="915" windowWidth="23895" windowHeight="11610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Legend and use" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="59">
   <si>
     <t>Bit Num</t>
   </si>
@@ -55,9 +55,6 @@
     <t>OvershootCountUse</t>
   </si>
   <si>
-    <t>AllowOutOfRangeInterimPID</t>
-  </si>
-  <si>
     <t>AllowExtraStabilityWait</t>
   </si>
   <si>
@@ -184,17 +181,56 @@
     <t>Enter 1 in each option cell in col. D you want to activate</t>
   </si>
   <si>
-    <t>Cell E1 has the number to punch in command 130.15 F1.</t>
-  </si>
-  <si>
-    <t>Column D will have 1's for the options in effect</t>
+    <t>DisAllowOutOfRangeInterimPID</t>
+  </si>
+  <si>
+    <t>UseSmoothedPositionForRamp</t>
+  </si>
+  <si>
+    <t>Apply_nY_min_fix</t>
+  </si>
+  <si>
+    <t>Include_P_and_D_in_bias</t>
+  </si>
+  <si>
+    <t>Cell E1 has the number to punch in command 130.15.</t>
+  </si>
+  <si>
+    <t>Enter options from 129.15 into D1. Column D will have 1's for the options in effect</t>
+  </si>
+  <si>
+    <t>Other parameters in {129,130}.15</t>
+  </si>
+  <si>
+    <t>PAdjust Recalc Scale2: inconsistent 16 in AP, PADJ_INC_RATIO=16 in ESD</t>
+  </si>
+  <si>
+    <t>PAdjust Recalc Scale: inconsistent 20 in AP, PADJ_INC_RATIO=16 in ESD</t>
+  </si>
+  <si>
+    <t>Low Overshoot Threshold: 4 in AP, OVERSHOOT_LOW=3 in ESD</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Min Number Of Ramp Points: 7 in AP, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>10 in ESD</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,8 +269,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -271,8 +314,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -280,11 +329,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -293,9 +362,23 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -576,55 +659,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{379C3635-3FB2-4EC1-BCDD-874929F6FD83}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="1" max="1" width="76.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -634,15 +742,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28" customWidth="1"/>
+    <col min="1" max="1" width="33.5703125" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" customWidth="1"/>
     <col min="7" max="7" width="71.42578125" customWidth="1"/>
     <col min="8" max="8" width="58.85546875" customWidth="1"/>
@@ -650,17 +758,17 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E1" s="3">
-        <f>SUMPRODUCT(C3:C34, E3:E34)</f>
-        <v>136</v>
+        <f>SUMPRODUCT(C3:C35, E3:E35)</f>
+        <v>32904</v>
       </c>
       <c r="F1" s="4">
         <v>1348</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -680,347 +788,428 @@
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="11">
         <v>0</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="11">
         <f>_xlfn.BITLSHIFT(1, B3)</f>
         <v>1</v>
       </c>
-      <c r="D3" t="str">
+      <c r="D3" s="11" t="str">
         <f>DEC2HEX(C3,4)</f>
         <v>0001</v>
       </c>
-      <c r="F3" t="str">
+      <c r="F3" s="11" t="str">
         <f>IF(_xlfn.BITAND(F$1,C3)&gt;0,1,"")</f>
         <v/>
       </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
+      <c r="G3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="12">
         <v>1</v>
       </c>
-      <c r="C4">
-        <f t="shared" ref="C4:C15" si="0">_xlfn.BITLSHIFT(1, B4)</f>
+      <c r="C4" s="12">
+        <f t="shared" ref="C4:C16" si="0">_xlfn.BITLSHIFT(1, B4)</f>
         <v>2</v>
       </c>
-      <c r="D4" t="str">
-        <f t="shared" ref="D4:D15" si="1">DEC2HEX(C4,4)</f>
+      <c r="D4" s="12" t="str">
+        <f t="shared" ref="D4:D16" si="1">DEC2HEX(C4,4)</f>
         <v>0002</v>
       </c>
-      <c r="F4" t="str">
+      <c r="F4" s="12" t="str">
         <f>IF(_xlfn.BITAND(F$1,C4)&gt;0,1,"")</f>
         <v/>
       </c>
-      <c r="G4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
+      <c r="G4" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="8">
         <v>2</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="8">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D5" t="str">
+      <c r="D5" s="8" t="str">
         <f t="shared" si="1"/>
         <v>0004</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="8">
         <f>IF(_xlfn.BITAND(F$1,C5)&gt;0,1,"")</f>
         <v>1</v>
       </c>
-      <c r="G5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
+      <c r="G5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="11">
         <v>3</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="11">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="D6" t="str">
+      <c r="D6" s="15" t="str">
         <f t="shared" si="1"/>
         <v>0008</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="11">
         <v>1</v>
       </c>
-      <c r="F6" t="str">
-        <f t="shared" ref="F6:F15" si="2">IF(_xlfn.BITAND(F$1,C6)&gt;0,1,"")</f>
+      <c r="F6" s="11" t="str">
+        <f t="shared" ref="F6:F16" si="2">IF(_xlfn.BITAND(F$1,C6)&gt;0,1,"")</f>
         <v/>
       </c>
-      <c r="G6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
+      <c r="G6" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="12">
         <v>4</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="12">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="D7" t="str">
+      <c r="D7" s="12" t="str">
         <f t="shared" si="1"/>
         <v>0010</v>
       </c>
-      <c r="F7" t="str">
+      <c r="F7" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="G7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8">
+      <c r="G7" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="12">
         <v>5</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="12">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="D8" t="str">
+      <c r="D8" s="12" t="str">
         <f t="shared" si="1"/>
         <v>0020</v>
       </c>
-      <c r="F8" t="str">
+      <c r="F8" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="G8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9">
+      <c r="G8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="20">
         <v>6</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="20">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="D9" t="str">
+      <c r="D9" s="20" t="str">
         <f t="shared" si="1"/>
         <v>0040</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="20">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="G9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10">
+      <c r="G9" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="12">
         <v>7</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="12">
         <f t="shared" si="0"/>
         <v>128</v>
       </c>
-      <c r="D10" t="str">
+      <c r="D10" s="12" t="str">
         <f t="shared" si="1"/>
         <v>0080</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="12">
         <v>1</v>
       </c>
-      <c r="F10" t="str">
+      <c r="F10" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="G10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11">
+      <c r="G10" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="12">
         <v>8</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="12">
         <f t="shared" si="0"/>
         <v>256</v>
       </c>
-      <c r="D11" t="str">
+      <c r="D11" s="12" t="str">
         <f t="shared" si="1"/>
         <v>0100</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="12">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="G11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12">
+      <c r="G11" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="12">
         <v>9</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="12">
         <f t="shared" si="0"/>
         <v>512</v>
       </c>
-      <c r="D12" t="str">
+      <c r="D12" s="12" t="str">
         <f t="shared" si="1"/>
         <v>0200</v>
       </c>
-      <c r="F12" t="str">
+      <c r="F12" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="G12" t="s">
-        <v>23</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="G12" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13">
+      <c r="B13" s="8">
         <v>10</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="8">
         <f t="shared" si="0"/>
         <v>1024</v>
       </c>
-      <c r="D13" t="str">
+      <c r="D13" s="8" t="str">
         <f t="shared" si="1"/>
         <v>0400</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="8">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="H13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14">
+      <c r="B14" s="11">
         <v>11</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="11">
+        <f t="shared" ref="C14" si="3">_xlfn.BITLSHIFT(1, B14)</f>
+        <v>2048</v>
+      </c>
+      <c r="D14" s="11" t="str">
+        <f t="shared" ref="D14" si="4">DEC2HEX(C14,4)</f>
+        <v>0800</v>
+      </c>
+      <c r="F14" s="11" t="str">
+        <f t="shared" ref="F14" si="5">IF(_xlfn.BITAND(F$1,C14)&gt;0,1,"")</f>
+        <v/>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="11">
+        <v>12</v>
+      </c>
+      <c r="C15" s="11">
         <f t="shared" si="0"/>
-        <v>2048</v>
-      </c>
-      <c r="D14" t="str">
+        <v>4096</v>
+      </c>
+      <c r="D15" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0800</v>
-      </c>
-      <c r="F14" t="str">
+        <v>1000</v>
+      </c>
+      <c r="F15" s="11" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="G14" t="s">
-        <v>36</v>
-      </c>
-      <c r="H14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15">
-        <v>12</v>
-      </c>
-      <c r="C15">
+      <c r="G15" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="12">
+        <v>13</v>
+      </c>
+      <c r="C16" s="12">
         <f t="shared" si="0"/>
-        <v>4096</v>
-      </c>
-      <c r="D15" t="str">
+        <v>8192</v>
+      </c>
+      <c r="D16" s="12" t="str">
         <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-      <c r="F15" t="str">
+        <v>2000</v>
+      </c>
+      <c r="F16" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="G15" t="s">
-        <v>42</v>
-      </c>
-      <c r="H15" t="s">
+      <c r="G16" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="12">
+        <v>14</v>
+      </c>
+      <c r="C17" s="12">
+        <f t="shared" ref="C17" si="6">_xlfn.BITLSHIFT(1, B17)</f>
+        <v>16384</v>
+      </c>
+      <c r="D17" s="12" t="str">
+        <f t="shared" ref="D17" si="7">DEC2HEX(C17,4)</f>
+        <v>4000</v>
+      </c>
+      <c r="F17" s="12" t="str">
+        <f t="shared" ref="F17" si="8">IF(_xlfn.BITAND(F$1,C17)&gt;0,1,"")</f>
+        <v/>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="12">
+        <v>15</v>
+      </c>
+      <c r="C18" s="12">
+        <f t="shared" ref="C18" si="9">_xlfn.BITLSHIFT(1, B18)</f>
+        <v>32768</v>
+      </c>
+      <c r="D18" s="12" t="str">
+        <f t="shared" ref="D18" si="10">DEC2HEX(C18,4)</f>
+        <v>8000</v>
+      </c>
+      <c r="E18" s="12">
+        <v>1</v>
+      </c>
+      <c r="F18" s="12" t="str">
+        <f t="shared" ref="F18" si="11">IF(_xlfn.BITAND(F$1,C18)&gt;0,1,"")</f>
+        <v/>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="12" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Attempted to remove position spikes on fill. More consistent tuning and control. (Default) tune options optimized - experimentally on Varipak and a springless DA valve Improved types of some variables
git-tfs-id: [http://szvptemfou01:8080/tfs/DefaultCollection]$/FW SVI FF Releases/Release3/FIRMWARE;C95517
</commit_message>
<xml_diff>
--- a/FIRMWARE/tasks/control/TuneStudyOptions.xlsx
+++ b/FIRMWARE/tasks/control/TuneStudyOptions.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\204061827\TFSSC\Workspaces\FW_SVI_FF_Releases\Release3\FIRMWARE\tasks\control\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\204061827\TFS\SVIFF_Releases\Release3\FIRMWARE\tasks\control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9854255-B3C5-415E-90DF-0E2C71715606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="915" windowWidth="23895" windowHeight="11610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="915" windowWidth="20940" windowHeight="6435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Legend and use" sheetId="2" r:id="rId1"/>
     <sheet name="Description and calc" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="64">
   <si>
     <t>Bit Num</t>
   </si>
@@ -85,9 +84,6 @@
     <t>1=like ESD, 0=like AP</t>
   </si>
   <si>
-    <t>1=interim tries are not range-limited</t>
-  </si>
-  <si>
     <t>1=In initial stabilization effort, add wait for stable position</t>
   </si>
   <si>
@@ -155,9 +151,6 @@
   </si>
   <si>
     <t xml:space="preserve">Doesn't appear to improve results </t>
-  </si>
-  <si>
-    <t>Provides a small stabilize effort. Slows the procees down</t>
   </si>
   <si>
     <t>1=Update poscomp along with other parameters</t>
@@ -225,12 +218,33 @@
       <t>10 in ESD</t>
     </r>
   </si>
+  <si>
+    <t>1=interim tries are range-limited</t>
+  </si>
+  <si>
+    <t>1=Account for valve moving in eval of bias</t>
+  </si>
+  <si>
+    <t>1= fix from ESD, 0 = like AP (logically wrong)</t>
+  </si>
+  <si>
+    <t>N/A for DA. Provides a small stabilize effort. Slows the procees down</t>
+  </si>
+  <si>
+    <t>Appears essential for DA, at least springless</t>
+  </si>
+  <si>
+    <t>Looks bad for DA. Provides a small stabilize effort. Slows the procees down</t>
+  </si>
+  <si>
+    <t>Looks essential for springless DA</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -276,8 +290,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -320,6 +342,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -353,7 +381,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -369,8 +397,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -379,6 +405,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,10 +688,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{379C3635-3FB2-4EC1-BCDD-874929F6FD83}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -672,67 +702,67 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
-        <v>58</v>
+      <c r="A12" s="20" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -741,11 +771,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,17 +788,17 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E1" s="3">
-        <f>SUMPRODUCT(C3:C35, E3:E35)</f>
-        <v>32904</v>
+        <f>SUMPRODUCT(C3:C19, E3:E19)</f>
+        <v>24742</v>
       </c>
       <c r="F1" s="4">
-        <v>1348</v>
+        <v>24598</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -788,13 +818,13 @@
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -820,12 +850,12 @@
         <v>15</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
-        <v>48</v>
+      <c r="A4" s="19" t="s">
+        <v>46</v>
       </c>
       <c r="B4" s="12">
         <v>1</v>
@@ -838,19 +868,22 @@
         <f t="shared" ref="D4:D16" si="1">DEC2HEX(C4,4)</f>
         <v>0002</v>
       </c>
-      <c r="F4" s="12" t="str">
+      <c r="E4" s="12">
+        <v>1</v>
+      </c>
+      <c r="F4" s="12">
         <f>IF(_xlfn.BITAND(F$1,C4)&gt;0,1,"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="21" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="8">
@@ -864,19 +897,22 @@
         <f t="shared" si="1"/>
         <v>0004</v>
       </c>
+      <c r="E5" s="8">
+        <v>1</v>
+      </c>
       <c r="F5" s="8">
         <f>IF(_xlfn.BITAND(F$1,C5)&gt;0,1,"")</f>
         <v>1</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="11">
@@ -886,23 +922,20 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="D6" s="15" t="str">
+      <c r="D6" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0008</v>
-      </c>
-      <c r="E6" s="11">
-        <v>1</v>
       </c>
       <c r="F6" s="11" t="str">
         <f t="shared" ref="F6:F16" si="2">IF(_xlfn.BITAND(F$1,C6)&gt;0,1,"")</f>
         <v/>
       </c>
       <c r="G6" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="12">
@@ -916,19 +949,19 @@
         <f t="shared" si="1"/>
         <v>0010</v>
       </c>
-      <c r="F7" s="12" t="str">
+      <c r="F7" s="12">
         <f t="shared" si="2"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="14" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="12">
@@ -942,45 +975,48 @@
         <f t="shared" si="1"/>
         <v>0020</v>
       </c>
+      <c r="E8" s="12">
+        <v>1</v>
+      </c>
       <c r="F8" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G8" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="20">
+      <c r="B9" s="18">
         <v>6</v>
       </c>
-      <c r="C9" s="20">
+      <c r="C9" s="18">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="D9" s="20" t="str">
+      <c r="D9" s="18" t="str">
         <f t="shared" si="1"/>
         <v>0040</v>
       </c>
-      <c r="F9" s="20">
+      <c r="F9" s="18" t="str">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G9" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="H9" s="20" t="s">
-        <v>28</v>
+        <v/>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="23" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="12">
@@ -1002,11 +1038,14 @@
         <v/>
       </c>
       <c r="G10" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="14" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="12">
@@ -1020,16 +1059,16 @@
         <f t="shared" si="1"/>
         <v>0100</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="12" t="str">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="G11" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="15" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="12">
@@ -1048,15 +1087,15 @@
         <v/>
       </c>
       <c r="G12" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" s="8">
         <v>10</v>
@@ -1069,20 +1108,20 @@
         <f t="shared" si="1"/>
         <v>0400</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="8" t="str">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="G13" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
         <v>35</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
-        <v>36</v>
       </c>
       <c r="B14" s="11">
         <v>11</v>
@@ -1100,15 +1139,15 @@
         <v/>
       </c>
       <c r="G14" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
-        <v>49</v>
+      <c r="A15" s="16" t="s">
+        <v>47</v>
       </c>
       <c r="B15" s="11">
         <v>12</v>
@@ -1126,15 +1165,15 @@
         <v/>
       </c>
       <c r="G15" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
-        <v>38</v>
+      <c r="A16" s="24" t="s">
+        <v>37</v>
       </c>
       <c r="B16" s="12">
         <v>13</v>
@@ -1147,20 +1186,23 @@
         <f t="shared" si="1"/>
         <v>2000</v>
       </c>
-      <c r="F16" s="12" t="str">
+      <c r="E16" s="12">
+        <v>1</v>
+      </c>
+      <c r="F16" s="12">
         <f t="shared" si="2"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
-        <v>50</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>48</v>
       </c>
       <c r="B17" s="12">
         <v>14</v>
@@ -1173,20 +1215,20 @@
         <f t="shared" ref="D17" si="7">DEC2HEX(C17,4)</f>
         <v>4000</v>
       </c>
-      <c r="F17" s="12" t="str">
+      <c r="E17" s="12">
+        <v>1</v>
+      </c>
+      <c r="F17" s="12">
         <f t="shared" ref="F17" si="8">IF(_xlfn.BITAND(F$1,C17)&gt;0,1,"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H17" s="12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
-        <v>51</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="22" t="s">
+        <v>49</v>
       </c>
       <c r="B18" s="12">
         <v>15</v>
@@ -1199,18 +1241,12 @@
         <f t="shared" ref="D18" si="10">DEC2HEX(C18,4)</f>
         <v>8000</v>
       </c>
-      <c r="E18" s="12">
-        <v>1</v>
-      </c>
       <c r="F18" s="12" t="str">
         <f t="shared" ref="F18" si="11">IF(_xlfn.BITAND(F$1,C18)&gt;0,1,"")</f>
         <v/>
       </c>
       <c r="G18" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" s="12" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>